<commit_message>
Added selectors to expand the identification of elements containing an image to include elements with a data-background attribute whose value ends in ".jpg", ".gif", or ".png", and elements with a style attribute whose value starts with "background:url".
</commit_message>
<xml_diff>
--- a/data/element data.xlsx
+++ b/data/element data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CutestPaw Correct" sheetId="8" r:id="rId1"/>
@@ -3499,7 +3499,7 @@
         <v>61</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E65" si="0">B5-SUM(C5:D5)</f>
+        <f t="shared" ref="E5:E64" si="0">B5-SUM(C5:D5)</f>
         <v>0</v>
       </c>
       <c r="G5" t="s">
@@ -9984,11 +9984,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:H306"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E277" sqref="E277"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10019,7 +10018,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>196</v>
       </c>
@@ -10042,7 +10041,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -10065,7 +10064,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -10088,7 +10087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -10111,7 +10110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -10134,7 +10133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>296</v>
       </c>
@@ -10157,7 +10156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -10180,7 +10179,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>192</v>
       </c>
@@ -10203,7 +10202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -10226,7 +10225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>252</v>
       </c>
@@ -10249,7 +10248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>390</v>
       </c>
@@ -10272,7 +10271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>486</v>
       </c>
@@ -10295,7 +10294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>490</v>
       </c>
@@ -10318,7 +10317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>248</v>
       </c>
@@ -10341,7 +10340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>257</v>
       </c>
@@ -10364,7 +10363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -10387,7 +10386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>191</v>
       </c>
@@ -10410,7 +10409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>482</v>
       </c>
@@ -10433,7 +10432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>232</v>
       </c>
@@ -10456,7 +10455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>297</v>
       </c>
@@ -10479,7 +10478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -10502,7 +10501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>204</v>
       </c>
@@ -10525,7 +10524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>398</v>
       </c>
@@ -10548,7 +10547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>405</v>
       </c>
@@ -10571,7 +10570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>406</v>
       </c>
@@ -10594,7 +10593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>478</v>
       </c>
@@ -10617,7 +10616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>358</v>
       </c>
@@ -10640,7 +10639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>361</v>
       </c>
@@ -10663,7 +10662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>370</v>
       </c>
@@ -10686,7 +10685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>384</v>
       </c>
@@ -10709,7 +10708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>399</v>
       </c>
@@ -10732,7 +10731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>407</v>
       </c>
@@ -10755,7 +10754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>408</v>
       </c>
@@ -10778,7 +10777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>412</v>
       </c>
@@ -10801,7 +10800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>415</v>
       </c>
@@ -10824,7 +10823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>440</v>
       </c>
@@ -10847,7 +10846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>453</v>
       </c>
@@ -10870,7 +10869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>253</v>
       </c>
@@ -10893,7 +10892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>256</v>
       </c>
@@ -10916,7 +10915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>456</v>
       </c>
@@ -10939,7 +10938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>458</v>
       </c>
@@ -10962,7 +10961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>462</v>
       </c>
@@ -10985,7 +10984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>463</v>
       </c>
@@ -11008,7 +11007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>472</v>
       </c>
@@ -11031,7 +11030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>473</v>
       </c>
@@ -11054,7 +11053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>474</v>
       </c>
@@ -11077,7 +11076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>475</v>
       </c>
@@ -11100,7 +11099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>476</v>
       </c>
@@ -11123,7 +11122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>498</v>
       </c>
@@ -11146,7 +11145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>194</v>
       </c>
@@ -11169,7 +11168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -11192,7 +11191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>335</v>
       </c>
@@ -11215,7 +11214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>338</v>
       </c>
@@ -11238,7 +11237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>197</v>
       </c>
@@ -11261,7 +11260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>363</v>
       </c>
@@ -11284,7 +11283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>387</v>
       </c>
@@ -11307,7 +11306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>496</v>
       </c>
@@ -11330,7 +11329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>238</v>
       </c>
@@ -11353,7 +11352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -11376,7 +11375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>247</v>
       </c>
@@ -11399,7 +11398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>249</v>
       </c>
@@ -11422,7 +11421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>254</v>
       </c>
@@ -11445,7 +11444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -11468,7 +11467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>344</v>
       </c>
@@ -11514,7 +11513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>202</v>
       </c>
@@ -11537,7 +11536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>345</v>
       </c>
@@ -11560,7 +11559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>347</v>
       </c>
@@ -11583,7 +11582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>348</v>
       </c>
@@ -11606,7 +11605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>349</v>
       </c>
@@ -11629,7 +11628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -11652,7 +11651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>357</v>
       </c>
@@ -11675,7 +11674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>362</v>
       </c>
@@ -11698,7 +11697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>376</v>
       </c>
@@ -11721,7 +11720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>394</v>
       </c>
@@ -11744,7 +11743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>452</v>
       </c>
@@ -11767,7 +11766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>494</v>
       </c>
@@ -11790,7 +11789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>501</v>
       </c>
@@ -11813,7 +11812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>233</v>
       </c>
@@ -11836,7 +11835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>234</v>
       </c>
@@ -11859,7 +11858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>235</v>
       </c>
@@ -11882,7 +11881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>236</v>
       </c>
@@ -11905,7 +11904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>203</v>
       </c>
@@ -11928,7 +11927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>237</v>
       </c>
@@ -11951,7 +11950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>239</v>
       </c>
@@ -11974,7 +11973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>240</v>
       </c>
@@ -11997,7 +11996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>241</v>
       </c>
@@ -12020,7 +12019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>242</v>
       </c>
@@ -12043,7 +12042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>243</v>
       </c>
@@ -12066,7 +12065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>244</v>
       </c>
@@ -12089,7 +12088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>245</v>
       </c>
@@ -12112,7 +12111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>246</v>
       </c>
@@ -12135,7 +12134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>189</v>
       </c>
@@ -12158,7 +12157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>250</v>
       </c>
@@ -12181,7 +12180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>251</v>
       </c>
@@ -12204,7 +12203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>255</v>
       </c>
@@ -12227,7 +12226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -12250,7 +12249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>206</v>
       </c>
@@ -12273,7 +12272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>260</v>
       </c>
@@ -12296,7 +12295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>261</v>
       </c>
@@ -12319,7 +12318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>262</v>
       </c>
@@ -12342,7 +12341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>263</v>
       </c>
@@ -12365,7 +12364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>264</v>
       </c>
@@ -12388,7 +12387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>265</v>
       </c>
@@ -12411,7 +12410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>266</v>
       </c>
@@ -12434,7 +12433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>267</v>
       </c>
@@ -12457,7 +12456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>268</v>
       </c>
@@ -12480,7 +12479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>269</v>
       </c>
@@ -12503,7 +12502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>270</v>
       </c>
@@ -12526,7 +12525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>271</v>
       </c>
@@ -12549,7 +12548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>272</v>
       </c>
@@ -12572,7 +12571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>273</v>
       </c>
@@ -12595,7 +12594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>274</v>
       </c>
@@ -12618,7 +12617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>275</v>
       </c>
@@ -12641,7 +12640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>276</v>
       </c>
@@ -12664,7 +12663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>277</v>
       </c>
@@ -12687,7 +12686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -12710,7 +12709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>279</v>
       </c>
@@ -12733,7 +12732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>280</v>
       </c>
@@ -12756,7 +12755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>281</v>
       </c>
@@ -12779,7 +12778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>282</v>
       </c>
@@ -12802,7 +12801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>283</v>
       </c>
@@ -12825,7 +12824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>284</v>
       </c>
@@ -12848,7 +12847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>285</v>
       </c>
@@ -12871,7 +12870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>286</v>
       </c>
@@ -12894,7 +12893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>287</v>
       </c>
@@ -12917,7 +12916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>288</v>
       </c>
@@ -12940,7 +12939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>289</v>
       </c>
@@ -12963,7 +12962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>290</v>
       </c>
@@ -12986,7 +12985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>291</v>
       </c>
@@ -13009,7 +13008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>292</v>
       </c>
@@ -13032,7 +13031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>293</v>
       </c>
@@ -13055,7 +13054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>294</v>
       </c>
@@ -13078,7 +13077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>298</v>
       </c>
@@ -13101,7 +13100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>299</v>
       </c>
@@ -13124,7 +13123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>300</v>
       </c>
@@ -13147,7 +13146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>301</v>
       </c>
@@ -13170,7 +13169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>302</v>
       </c>
@@ -13193,7 +13192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>303</v>
       </c>
@@ -13216,7 +13215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>304</v>
       </c>
@@ -13239,7 +13238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1">
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>305</v>
       </c>
@@ -13262,7 +13261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>306</v>
       </c>
@@ -13285,7 +13284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1">
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>307</v>
       </c>
@@ -13308,7 +13307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>308</v>
       </c>
@@ -13331,7 +13330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>309</v>
       </c>
@@ -13354,7 +13353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>310</v>
       </c>
@@ -13377,7 +13376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>311</v>
       </c>
@@ -13400,7 +13399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>312</v>
       </c>
@@ -13423,7 +13422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>313</v>
       </c>
@@ -13446,7 +13445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1">
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>314</v>
       </c>
@@ -13469,7 +13468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1">
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>315</v>
       </c>
@@ -13492,7 +13491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1">
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>316</v>
       </c>
@@ -13515,7 +13514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1">
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>317</v>
       </c>
@@ -13538,7 +13537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1">
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>318</v>
       </c>
@@ -13561,7 +13560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1">
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>319</v>
       </c>
@@ -13584,7 +13583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1">
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>320</v>
       </c>
@@ -13607,7 +13606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1">
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>321</v>
       </c>
@@ -13630,7 +13629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1">
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>322</v>
       </c>
@@ -13653,7 +13652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1">
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>323</v>
       </c>
@@ -13676,7 +13675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1">
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>324</v>
       </c>
@@ -13699,7 +13698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>325</v>
       </c>
@@ -13722,7 +13721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>326</v>
       </c>
@@ -13745,7 +13744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1">
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>327</v>
       </c>
@@ -13768,7 +13767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1">
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>328</v>
       </c>
@@ -13791,7 +13790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1">
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>329</v>
       </c>
@@ -13814,7 +13813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1">
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>330</v>
       </c>
@@ -13837,7 +13836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1">
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>331</v>
       </c>
@@ -13860,7 +13859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>332</v>
       </c>
@@ -13883,7 +13882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>333</v>
       </c>
@@ -13906,7 +13905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1">
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>334</v>
       </c>
@@ -13929,7 +13928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1">
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>336</v>
       </c>
@@ -13952,7 +13951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1">
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>337</v>
       </c>
@@ -13975,7 +13974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1">
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>339</v>
       </c>
@@ -13998,7 +13997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1">
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>340</v>
       </c>
@@ -14021,7 +14020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1">
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>341</v>
       </c>
@@ -14044,7 +14043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1">
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>342</v>
       </c>
@@ -14067,7 +14066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1">
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>343</v>
       </c>
@@ -14090,7 +14089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1">
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>346</v>
       </c>
@@ -14113,7 +14112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1">
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>184</v>
       </c>
@@ -14159,7 +14158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1">
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>351</v>
       </c>
@@ -14182,7 +14181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1">
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>352</v>
       </c>
@@ -14205,7 +14204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1">
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>353</v>
       </c>
@@ -14228,7 +14227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1">
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>185</v>
       </c>
@@ -14251,7 +14250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1">
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>354</v>
       </c>
@@ -14274,7 +14273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1">
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>355</v>
       </c>
@@ -14297,7 +14296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1">
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>356</v>
       </c>
@@ -14320,7 +14319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1">
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>12</v>
       </c>
@@ -14343,7 +14342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>359</v>
       </c>
@@ -14366,7 +14365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1">
+    <row r="193" spans="1:8">
       <c r="A193" t="s">
         <v>360</v>
       </c>
@@ -14389,7 +14388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1">
+    <row r="194" spans="1:8">
       <c r="A194" t="s">
         <v>364</v>
       </c>
@@ -14412,7 +14411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1">
+    <row r="195" spans="1:8">
       <c r="A195" t="s">
         <v>365</v>
       </c>
@@ -14435,7 +14434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1">
+    <row r="196" spans="1:8">
       <c r="A196" t="s">
         <v>366</v>
       </c>
@@ -14458,7 +14457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1">
+    <row r="197" spans="1:8">
       <c r="A197" t="s">
         <v>367</v>
       </c>
@@ -14481,7 +14480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1">
+    <row r="198" spans="1:8">
       <c r="A198" t="s">
         <v>368</v>
       </c>
@@ -14504,7 +14503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1">
+    <row r="199" spans="1:8">
       <c r="A199" t="s">
         <v>369</v>
       </c>
@@ -14527,7 +14526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1">
+    <row r="200" spans="1:8">
       <c r="A200" t="s">
         <v>371</v>
       </c>
@@ -14550,7 +14549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1">
+    <row r="201" spans="1:8">
       <c r="A201" t="s">
         <v>372</v>
       </c>
@@ -14573,7 +14572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1">
+    <row r="202" spans="1:8">
       <c r="A202" t="s">
         <v>373</v>
       </c>
@@ -14596,7 +14595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1">
+    <row r="203" spans="1:8">
       <c r="A203" t="s">
         <v>374</v>
       </c>
@@ -14619,7 +14618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1">
+    <row r="204" spans="1:8">
       <c r="A204" t="s">
         <v>375</v>
       </c>
@@ -14642,7 +14641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1">
+    <row r="205" spans="1:8">
       <c r="A205" t="s">
         <v>504</v>
       </c>
@@ -14665,7 +14664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1">
+    <row r="206" spans="1:8">
       <c r="A206" t="s">
         <v>505</v>
       </c>
@@ -14688,7 +14687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1">
+    <row r="207" spans="1:8">
       <c r="A207" t="s">
         <v>506</v>
       </c>
@@ -14711,7 +14710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1">
+    <row r="208" spans="1:8">
       <c r="A208" t="s">
         <v>377</v>
       </c>
@@ -14734,7 +14733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1">
+    <row r="209" spans="1:8">
       <c r="A209" t="s">
         <v>378</v>
       </c>
@@ -14757,7 +14756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1">
+    <row r="210" spans="1:8">
       <c r="A210" t="s">
         <v>379</v>
       </c>
@@ -14780,7 +14779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1">
+    <row r="211" spans="1:8">
       <c r="A211" t="s">
         <v>380</v>
       </c>
@@ -14803,7 +14802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1">
+    <row r="212" spans="1:8">
       <c r="A212" t="s">
         <v>381</v>
       </c>
@@ -14826,7 +14825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1">
+    <row r="213" spans="1:8">
       <c r="A213" t="s">
         <v>382</v>
       </c>
@@ -14849,7 +14848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1">
+    <row r="214" spans="1:8">
       <c r="A214" t="s">
         <v>383</v>
       </c>
@@ -14872,7 +14871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1">
+    <row r="215" spans="1:8">
       <c r="A215" t="s">
         <v>507</v>
       </c>
@@ -14895,7 +14894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1">
+    <row r="216" spans="1:8">
       <c r="A216" t="s">
         <v>385</v>
       </c>
@@ -14918,7 +14917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:8" hidden="1">
+    <row r="217" spans="1:8">
       <c r="A217" t="s">
         <v>386</v>
       </c>
@@ -14941,7 +14940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1">
+    <row r="218" spans="1:8">
       <c r="A218" t="s">
         <v>388</v>
       </c>
@@ -14964,7 +14963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1">
+    <row r="219" spans="1:8">
       <c r="A219" t="s">
         <v>389</v>
       </c>
@@ -14987,7 +14986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1">
+    <row r="220" spans="1:8">
       <c r="A220" t="s">
         <v>391</v>
       </c>
@@ -15010,7 +15009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1">
+    <row r="221" spans="1:8">
       <c r="A221" t="s">
         <v>392</v>
       </c>
@@ -15033,7 +15032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:8" hidden="1">
+    <row r="222" spans="1:8">
       <c r="A222" t="s">
         <v>393</v>
       </c>
@@ -15056,7 +15055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1">
+    <row r="223" spans="1:8">
       <c r="A223" t="s">
         <v>395</v>
       </c>
@@ -15079,7 +15078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1">
+    <row r="224" spans="1:8">
       <c r="A224" t="s">
         <v>396</v>
       </c>
@@ -15102,7 +15101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1">
+    <row r="225" spans="1:8">
       <c r="A225" t="s">
         <v>397</v>
       </c>
@@ -15125,7 +15124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1">
+    <row r="226" spans="1:8">
       <c r="A226" t="s">
         <v>400</v>
       </c>
@@ -15148,7 +15147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1">
+    <row r="227" spans="1:8">
       <c r="A227" t="s">
         <v>401</v>
       </c>
@@ -15171,7 +15170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1">
+    <row r="228" spans="1:8">
       <c r="A228" t="s">
         <v>402</v>
       </c>
@@ -15194,7 +15193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1">
+    <row r="229" spans="1:8">
       <c r="A229" t="s">
         <v>403</v>
       </c>
@@ -15217,7 +15216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1">
+    <row r="230" spans="1:8">
       <c r="A230" t="s">
         <v>404</v>
       </c>
@@ -15240,7 +15239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1">
+    <row r="231" spans="1:8">
       <c r="A231" t="s">
         <v>409</v>
       </c>
@@ -15263,7 +15262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1">
+    <row r="232" spans="1:8">
       <c r="A232" t="s">
         <v>410</v>
       </c>
@@ -15286,7 +15285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1">
+    <row r="233" spans="1:8">
       <c r="A233" t="s">
         <v>411</v>
       </c>
@@ -15309,7 +15308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1">
+    <row r="234" spans="1:8">
       <c r="A234" t="s">
         <v>413</v>
       </c>
@@ -15332,7 +15331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1">
+    <row r="235" spans="1:8">
       <c r="A235" t="s">
         <v>414</v>
       </c>
@@ -15355,7 +15354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1">
+    <row r="236" spans="1:8">
       <c r="A236" t="s">
         <v>416</v>
       </c>
@@ -15378,7 +15377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1">
+    <row r="237" spans="1:8">
       <c r="A237" t="s">
         <v>417</v>
       </c>
@@ -15401,7 +15400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1">
+    <row r="238" spans="1:8">
       <c r="A238" t="s">
         <v>418</v>
       </c>
@@ -15424,7 +15423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1">
+    <row r="239" spans="1:8">
       <c r="A239" t="s">
         <v>419</v>
       </c>
@@ -15447,7 +15446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1">
+    <row r="240" spans="1:8">
       <c r="A240" t="s">
         <v>420</v>
       </c>
@@ -15470,7 +15469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:8" hidden="1">
+    <row r="241" spans="1:8">
       <c r="A241" t="s">
         <v>421</v>
       </c>
@@ -15493,7 +15492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:8" hidden="1">
+    <row r="242" spans="1:8">
       <c r="A242" t="s">
         <v>422</v>
       </c>
@@ -15516,7 +15515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1">
+    <row r="243" spans="1:8">
       <c r="A243" t="s">
         <v>423</v>
       </c>
@@ -15539,7 +15538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1">
+    <row r="244" spans="1:8">
       <c r="A244" t="s">
         <v>424</v>
       </c>
@@ -15562,7 +15561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1">
+    <row r="245" spans="1:8">
       <c r="A245" t="s">
         <v>425</v>
       </c>
@@ -15585,7 +15584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1">
+    <row r="246" spans="1:8">
       <c r="A246" t="s">
         <v>426</v>
       </c>
@@ -15608,7 +15607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1">
+    <row r="247" spans="1:8">
       <c r="A247" t="s">
         <v>427</v>
       </c>
@@ -15631,7 +15630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1">
+    <row r="248" spans="1:8">
       <c r="A248" t="s">
         <v>428</v>
       </c>
@@ -15654,7 +15653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1">
+    <row r="249" spans="1:8">
       <c r="A249" t="s">
         <v>429</v>
       </c>
@@ -15677,7 +15676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1">
+    <row r="250" spans="1:8">
       <c r="A250" t="s">
         <v>430</v>
       </c>
@@ -15700,7 +15699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1">
+    <row r="251" spans="1:8">
       <c r="A251" t="s">
         <v>431</v>
       </c>
@@ -15723,7 +15722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1">
+    <row r="252" spans="1:8">
       <c r="A252" t="s">
         <v>432</v>
       </c>
@@ -15746,7 +15745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1">
+    <row r="253" spans="1:8">
       <c r="A253" t="s">
         <v>433</v>
       </c>
@@ -15769,7 +15768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:8" hidden="1">
+    <row r="254" spans="1:8">
       <c r="A254" t="s">
         <v>434</v>
       </c>
@@ -15792,7 +15791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1">
+    <row r="255" spans="1:8">
       <c r="A255" t="s">
         <v>435</v>
       </c>
@@ -15815,7 +15814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1">
+    <row r="256" spans="1:8">
       <c r="A256" t="s">
         <v>436</v>
       </c>
@@ -15838,7 +15837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1">
+    <row r="257" spans="1:8">
       <c r="A257" t="s">
         <v>437</v>
       </c>
@@ -15861,7 +15860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:8" hidden="1">
+    <row r="258" spans="1:8">
       <c r="A258" t="s">
         <v>438</v>
       </c>
@@ -15884,7 +15883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1">
+    <row r="259" spans="1:8">
       <c r="A259" t="s">
         <v>439</v>
       </c>
@@ -15907,7 +15906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1">
+    <row r="260" spans="1:8">
       <c r="A260" t="s">
         <v>441</v>
       </c>
@@ -15930,7 +15929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:8" hidden="1">
+    <row r="261" spans="1:8">
       <c r="A261" t="s">
         <v>442</v>
       </c>
@@ -15953,7 +15952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:8" hidden="1">
+    <row r="262" spans="1:8">
       <c r="A262" t="s">
         <v>443</v>
       </c>
@@ -15976,7 +15975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1">
+    <row r="263" spans="1:8">
       <c r="A263" t="s">
         <v>444</v>
       </c>
@@ -15999,7 +15998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1">
+    <row r="264" spans="1:8">
       <c r="A264" t="s">
         <v>445</v>
       </c>
@@ -16022,7 +16021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1">
+    <row r="265" spans="1:8">
       <c r="A265" t="s">
         <v>446</v>
       </c>
@@ -16045,7 +16044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1">
+    <row r="266" spans="1:8">
       <c r="A266" t="s">
         <v>447</v>
       </c>
@@ -16068,7 +16067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1">
+    <row r="267" spans="1:8">
       <c r="A267" t="s">
         <v>448</v>
       </c>
@@ -16091,7 +16090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1">
+    <row r="268" spans="1:8">
       <c r="A268" t="s">
         <v>449</v>
       </c>
@@ -16114,7 +16113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1">
+    <row r="269" spans="1:8">
       <c r="A269" t="s">
         <v>450</v>
       </c>
@@ -16137,7 +16136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:8" hidden="1">
+    <row r="270" spans="1:8">
       <c r="A270" t="s">
         <v>451</v>
       </c>
@@ -16160,7 +16159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:8" hidden="1">
+    <row r="271" spans="1:8">
       <c r="A271" t="s">
         <v>454</v>
       </c>
@@ -16183,7 +16182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1">
+    <row r="272" spans="1:8">
       <c r="A272" t="s">
         <v>455</v>
       </c>
@@ -16206,7 +16205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1">
+    <row r="273" spans="1:8">
       <c r="A273" t="s">
         <v>457</v>
       </c>
@@ -16229,7 +16228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1">
+    <row r="274" spans="1:8">
       <c r="A274" t="s">
         <v>459</v>
       </c>
@@ -16252,7 +16251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1">
+    <row r="275" spans="1:8">
       <c r="A275" t="s">
         <v>460</v>
       </c>
@@ -16344,7 +16343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1">
+    <row r="279" spans="1:8">
       <c r="A279" t="s">
         <v>464</v>
       </c>
@@ -16367,7 +16366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:8" hidden="1">
+    <row r="280" spans="1:8">
       <c r="A280" t="s">
         <v>465</v>
       </c>
@@ -16390,7 +16389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1">
+    <row r="281" spans="1:8">
       <c r="A281" t="s">
         <v>466</v>
       </c>
@@ -16413,7 +16412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1">
+    <row r="282" spans="1:8">
       <c r="A282" t="s">
         <v>467</v>
       </c>
@@ -16436,7 +16435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1">
+    <row r="283" spans="1:8">
       <c r="A283" t="s">
         <v>468</v>
       </c>
@@ -16459,7 +16458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1">
+    <row r="284" spans="1:8">
       <c r="A284" t="s">
         <v>469</v>
       </c>
@@ -16482,7 +16481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1">
+    <row r="285" spans="1:8">
       <c r="A285" t="s">
         <v>470</v>
       </c>
@@ -16505,7 +16504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1">
+    <row r="286" spans="1:8">
       <c r="A286" t="s">
         <v>471</v>
       </c>
@@ -16528,7 +16527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1">
+    <row r="287" spans="1:8">
       <c r="A287" t="s">
         <v>477</v>
       </c>
@@ -16551,7 +16550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1">
+    <row r="288" spans="1:8">
       <c r="A288" t="s">
         <v>479</v>
       </c>
@@ -16574,7 +16573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1">
+    <row r="289" spans="1:8">
       <c r="A289" t="s">
         <v>480</v>
       </c>
@@ -16597,7 +16596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1">
+    <row r="290" spans="1:8">
       <c r="A290" t="s">
         <v>481</v>
       </c>
@@ -16620,7 +16619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1">
+    <row r="291" spans="1:8">
       <c r="A291" t="s">
         <v>483</v>
       </c>
@@ -16643,7 +16642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1">
+    <row r="292" spans="1:8">
       <c r="A292" t="s">
         <v>484</v>
       </c>
@@ -16666,7 +16665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1">
+    <row r="293" spans="1:8">
       <c r="A293" t="s">
         <v>13</v>
       </c>
@@ -16689,7 +16688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1">
+    <row r="294" spans="1:8">
       <c r="A294" t="s">
         <v>485</v>
       </c>
@@ -16712,7 +16711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1">
+    <row r="295" spans="1:8">
       <c r="A295" t="s">
         <v>487</v>
       </c>
@@ -16735,7 +16734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1">
+    <row r="296" spans="1:8">
       <c r="A296" t="s">
         <v>488</v>
       </c>
@@ -16758,7 +16757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:8" hidden="1">
+    <row r="297" spans="1:8">
       <c r="A297" t="s">
         <v>489</v>
       </c>
@@ -16781,7 +16780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1">
+    <row r="298" spans="1:8">
       <c r="A298" t="s">
         <v>491</v>
       </c>
@@ -16804,7 +16803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1">
+    <row r="299" spans="1:8">
       <c r="A299" t="s">
         <v>492</v>
       </c>
@@ -16827,7 +16826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1">
+    <row r="300" spans="1:8">
       <c r="A300" t="s">
         <v>493</v>
       </c>
@@ -16850,7 +16849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1">
+    <row r="301" spans="1:8">
       <c r="A301" t="s">
         <v>495</v>
       </c>
@@ -16873,7 +16872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1">
+    <row r="302" spans="1:8">
       <c r="A302" t="s">
         <v>497</v>
       </c>
@@ -16896,7 +16895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8" hidden="1">
+    <row r="303" spans="1:8">
       <c r="A303" t="s">
         <v>499</v>
       </c>
@@ -16919,7 +16918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1">
+    <row r="304" spans="1:8">
       <c r="A304" t="s">
         <v>500</v>
       </c>
@@ -16942,7 +16941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1">
+    <row r="305" spans="1:8">
       <c r="A305" t="s">
         <v>502</v>
       </c>
@@ -16989,13 +16988,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E3:H306">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="E3:H306"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -17009,7 +17002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>